<commit_message>
Reworked Loading Sf7 Details
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf1.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="97">
   <si>
     <t>LRN</t>
   </si>
@@ -358,85 +358,37 @@
     <t>Crossing Bayabas National High School</t>
   </si>
   <si>
-    <t>2019-2020</t>
+    <t>2020-2021</t>
   </si>
   <si>
     <t>Grade 7</t>
   </si>
   <si>
-    <t xml:space="preserve"> FIDELITY</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>RIZAL</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t xml:space="preserve">FUMINO ONA FURAHASHI </t>
-  </si>
-  <si>
-    <t>123543457474</t>
-  </si>
-  <si>
-    <t>Paderogao, Phil Rey, E. Jr</t>
+    <t xml:space="preserve">PHIL REY ESTRELLAÑ PADEROGAO </t>
+  </si>
+  <si>
+    <t>123456789023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rizal, Jose </t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>2006-12-11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Manay, Davao Oriental</t>
-  </si>
-  <si>
-    <t>Mandaya</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Roman Catholic</t>
-  </si>
-  <si>
-    <t>Purok 18, Bato St.</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
-    <t>Manay</t>
-  </si>
-  <si>
-    <t>Davao Oriental</t>
-  </si>
-  <si>
-    <t>Enrique C. Paderogao</t>
-  </si>
-  <si>
-    <t>Jocelyn E. Paderogao</t>
-  </si>
-  <si>
-    <t>09483428056</t>
-  </si>
-  <si>
-    <t>YoloNew 1_7</t>
-  </si>
-  <si>
-    <t>123456789023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rizal, Jose </t>
-  </si>
-  <si>
     <t>2006-05-13</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>LOCATION</t>
@@ -475,7 +427,7 @@
     <t>CONTACT</t>
   </si>
   <si>
-    <t>Yolo 3_7</t>
+    <t>Yolo 3_9</t>
   </si>
 </sst>
 </file>
@@ -1680,97 +1632,59 @@
         <v>86</v>
       </c>
       <c r="I7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="K7" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="L7" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="M7" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="N7" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="O7" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="P7" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="P7" s="19" t="s">
-        <v>86</v>
-      </c>
       <c r="Q7" s="19" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q8" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S8" s="19" t="s">
-        <v>112</v>
-      </c>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="19"/>
     </row>
     <row r="9" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>

</xml_diff>

<commit_message>
Applied Thread Speeds From Settings.txt
-set Thread.Sleep() for threads speed from 100,50,25,0
-set Thread.Sleep() for pausing speed from 500,250,125,0
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf1.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="114">
   <si>
     <t>LRN</t>
   </si>
@@ -358,22 +358,22 @@
     <t>Crossing Bayabas National High School</t>
   </si>
   <si>
-    <t>2020-2021</t>
+    <t>2019-2020</t>
   </si>
   <si>
     <t>Grade 7</t>
   </si>
   <si>
-    <t>RIZAL</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>FIDELITY</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t xml:space="preserve">PHIL REY ESTRELLAÑ PADEROGAO </t>
+    <t xml:space="preserve">FUMINO ONA FURAHASHI </t>
   </si>
   <si>
     <t>123456789023</t>
@@ -388,7 +388,7 @@
     <t>2006-05-13</t>
   </si>
   <si>
-    <t>14</t>
+    <t>13</t>
   </si>
   <si>
     <t>LOCATION</t>
@@ -427,7 +427,58 @@
     <t>CONTACT</t>
   </si>
   <si>
-    <t>Yolo 3_9</t>
+    <t>Yolo 3_7</t>
+  </si>
+  <si>
+    <t>123543457474</t>
+  </si>
+  <si>
+    <t>Paderogao, Phil Rey, E. Jr</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>2006-12-11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Manay, Davao Oriental</t>
+  </si>
+  <si>
+    <t>Mandaya</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Roman Catholic</t>
+  </si>
+  <si>
+    <t>Purok 18, Bato St.</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Manay</t>
+  </si>
+  <si>
+    <t>Davao Oriental</t>
+  </si>
+  <si>
+    <t>Enrique C. Paderogao</t>
+  </si>
+  <si>
+    <t>Jocelyn E. Paderogao</t>
+  </si>
+  <si>
+    <t>09483428056</t>
+  </si>
+  <si>
+    <t>YoloNew 1_7</t>
   </si>
 </sst>
 </file>
@@ -1666,25 +1717,63 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="19"/>
+      <c r="A8" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>

</xml_diff>

<commit_message>
Mass Update on Registration and Forms
Registration System:
-Got reading excel file working
Forms System
-Updated Excel Files
-Fixed counting for female on SF1
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf1.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Forms System Final\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3971D2EE-25A7-43ED-83A1-D686E814C49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0930A725-BF01-45E5-8347-2CDAC4D339ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15120" firstSheet="2" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10 Pupils (0)" sheetId="3" r:id="rId1"/>
@@ -89,28 +89,6 @@
   </si>
   <si>
     <t>(Please refer to the legend in the last page)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NAME</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(last name, first name, middle name)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -343,6 +321,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NAME</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(last name, first name, middle name,extention)</t>
+    </r>
+  </si>
+  <si>
     <t>304356</t>
   </si>
   <si>
@@ -367,19 +367,19 @@
     <t>FIDELITY</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUMINO ONA FURAHASHI </t>
+    <t>FURAHASHI, FUMINO, ONA</t>
   </si>
   <si>
     <t>123456789023</t>
   </si>
   <si>
-    <t xml:space="preserve">Rizal, Jose </t>
+    <t>RIZAL, JOSE</t>
   </si>
   <si>
     <t>M</t>
@@ -433,7 +433,7 @@
     <t>123543457474</t>
   </si>
   <si>
-    <t>Paderogao, Phil Rey, E. Jr</t>
+    <t>PADEROGAO, PHIL REY, ESTRELLA, JR</t>
   </si>
   <si>
     <t>F</t>
@@ -794,7 +794,7 @@
       <alignment horizontal="distributed" vertical="distributed" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -895,6 +895,123 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -902,169 +1019,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1426,8 +1429,8 @@
   </sheetPr>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,108 +1456,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
     </row>
     <row r="3" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="87"/>
-      <c r="G3" s="79" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="80"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="88" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="89"/>
-      <c r="L3" s="79" t="s">
+      <c r="K3" s="42"/>
+      <c r="L3" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="80"/>
-      <c r="N3" s="81"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="37"/>
       <c r="P3" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
     </row>
     <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="39" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="40"/>
+      <c r="K4" s="47"/>
       <c r="L4" s="27" t="s">
         <v>73</v>
       </c>
       <c r="M4" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N4" s="27" t="s">
         <v>74</v>
@@ -1562,56 +1565,56 @@
       <c r="O4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="79" t="s">
+      <c r="P4" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="81"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="37"/>
     </row>
     <row r="5" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="D5" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="72" t="s">
+      <c r="H5" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="I5" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="62"/>
+      <c r="P5" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="78"/>
-      <c r="P5" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="53" t="s">
+      <c r="Q5" s="64"/>
+      <c r="R5" s="44" t="s">
         <v>21</v>
       </c>
       <c r="S5" s="5" t="s">
@@ -1619,15 +1622,15 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="75"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1655,7 @@
       <c r="Q6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="54"/>
+      <c r="R6" s="45"/>
       <c r="S6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1944,207 +1947,218 @@
       <c r="S16" s="19"/>
     </row>
     <row r="18" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="90" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
+      <c r="B18" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
       <c r="S18" s="6"/>
     </row>
     <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
+      <c r="C19" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="43"/>
+        <v>31</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="67"/>
+      <c r="K19" s="68"/>
       <c r="L19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N19" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="O19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R19" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="46"/>
+        <v>43</v>
+      </c>
+      <c r="I20" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M20" s="11" t="s">
         <v>76</v>
       </c>
       <c r="N20" s="13"/>
-      <c r="O20" s="37" t="s">
+      <c r="O20" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="P20" s="38"/>
+      <c r="P20" s="76"/>
       <c r="Q20" s="12"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
     </row>
     <row r="21" spans="1:20" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
+        <v>36</v>
+      </c>
+      <c r="C21" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="78"/>
       <c r="H21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="48"/>
-      <c r="K21" s="49"/>
+        <v>44</v>
+      </c>
+      <c r="I21" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="80"/>
+      <c r="K21" s="81"/>
       <c r="L21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N21" s="11"/>
-      <c r="O21" s="55" t="s">
+      <c r="O21" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="P21" s="83"/>
+      <c r="R21" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="P21" s="56"/>
-      <c r="R21" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="S21" s="57"/>
-      <c r="T21" s="57"/>
+      <c r="S21" s="84"/>
+      <c r="T21" s="84"/>
     </row>
     <row r="22" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="M22" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="N22" s="51"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="N22" s="87"/>
       <c r="O22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="P22" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="P22" s="24" t="s">
-        <v>63</v>
-      </c>
       <c r="R22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S22" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="S22" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="T22" s="50"/>
+      <c r="T22" s="72"/>
     </row>
     <row r="23" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="C23" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
       <c r="H23" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I23" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
+        <v>46</v>
+      </c>
+      <c r="I23" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="I20:K20"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:K4"/>
@@ -2161,25 +2175,14 @@
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Reworking Registration & Forms System
-Can now import different excel files
-Registration still not complete
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf1.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Forms System Final\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0930A725-BF01-45E5-8347-2CDAC4D339ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD021ABE-E591-4A86-B045-86DAD36BF482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15120" firstSheet="2" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="10 Pupils (0)" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="112">
   <si>
     <t>LRN</t>
   </si>
@@ -177,10 +177,6 @@
       <t xml:space="preserve">
 (If not parent)</t>
     </r>
-  </si>
-  <si>
-    <t>Birth 
-Place</t>
   </si>
   <si>
     <t>Region</t>
@@ -376,6 +372,9 @@
     <t>FURAHASHI, FUMINO, ONA</t>
   </si>
   <si>
+    <t>PHIL REY ESTRELLA PADEROGAO</t>
+  </si>
+  <si>
     <t>123456789023</t>
   </si>
   <si>
@@ -385,15 +384,12 @@
     <t>M</t>
   </si>
   <si>
-    <t>2006-05-13</t>
+    <t>05/13/2006</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>LOCATION</t>
-  </si>
-  <si>
     <t>LANGUAGE</t>
   </si>
   <si>
@@ -439,13 +435,10 @@
     <t>F</t>
   </si>
   <si>
-    <t>2006-12-11</t>
+    <t>12/11/2006</t>
   </si>
   <si>
     <t>12</t>
-  </si>
-  <si>
-    <t>Manay, Davao Oriental</t>
   </si>
   <si>
     <t>Mandaya</t>
@@ -895,6 +888,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,33 +903,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -943,18 +936,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1065,9 +1061,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1427,10 +1420,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,228 +1432,220 @@
     <col min="2" max="2" customWidth="true" style="1" width="27.42578125" collapsed="false"/>
     <col min="3" max="3" customWidth="true" style="1" width="4.140625" collapsed="false"/>
     <col min="4" max="4" customWidth="true" style="1" width="15.5703125" collapsed="false"/>
-    <col min="5" max="6" style="1" width="9.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="1" width="13.42578125" collapsed="false"/>
-    <col min="8" max="8" style="1" width="9.140625" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="1" width="11.140625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="1" width="13.42578125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" style="1" width="14.5703125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" style="1" width="15.7109375" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" style="1" width="18.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" style="1" width="17.7109375" collapsed="false"/>
-    <col min="18" max="19" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
-    <col min="20" max="16384" style="1" width="9.140625" collapsed="false"/>
+    <col min="5" max="5" style="1" width="9.140625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.42578125" collapsed="false"/>
+    <col min="7" max="7" style="1" width="9.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="1" width="11.140625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="1" width="13.42578125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="1" width="14.5703125" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="1" width="15.7109375" collapsed="false"/>
+    <col min="14" max="14" customWidth="true" style="1" width="18.42578125" collapsed="false"/>
+    <col min="15" max="15" customWidth="true" style="1" width="18.7109375" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="1" width="17.7109375" collapsed="false"/>
+    <col min="17" max="18" customWidth="true" style="1" width="12.7109375" collapsed="false"/>
+    <col min="19" max="16384" style="1" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
     </row>
-    <row r="3" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="39"/>
+      <c r="M3" s="38"/>
+      <c r="O3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="37"/>
-      <c r="P3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
-    <row r="4" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="47"/>
+      <c r="K4" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="O4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="37"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="38"/>
     </row>
-    <row r="5" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="91" t="s">
-        <v>67</v>
+      <c r="B5" s="50" t="s">
+        <v>66</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="54" t="s">
+      <c r="D5" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="56" t="s">
+      <c r="F5" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="G5" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="H5" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="I5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="60" t="s">
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="62"/>
-      <c r="P5" s="63" t="s">
+      <c r="N5" s="63"/>
+      <c r="O5" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="44" t="s">
+      <c r="P5" s="65"/>
+      <c r="Q5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="51"/>
       <c r="C6" s="53"/>
       <c r="D6" s="51"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="4" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="K6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="4" t="s">
+      <c r="Q6" s="44"/>
+      <c r="R6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>79</v>
       </c>
@@ -1683,10 +1668,10 @@
         <v>85</v>
       </c>
       <c r="H7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>12</v>
       </c>
       <c r="J7" s="19" t="s">
         <v>87</v>
@@ -1709,76 +1694,70 @@
       <c r="P7" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="R7" s="17" t="s">
+      <c r="R7" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="S7" s="19" t="s">
+    </row>
+    <row r="8" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>96</v>
       </c>
+      <c r="B8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q8" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="R8" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="S8" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -1795,11 +1774,10 @@
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="19"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="19"/>
     </row>
-    <row r="10" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -1816,11 +1794,10 @@
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="19"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="19"/>
     </row>
-    <row r="11" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1837,11 +1814,10 @@
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="19"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="19"/>
     </row>
-    <row r="12" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1858,11 +1834,10 @@
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="19"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="19"/>
     </row>
-    <row r="13" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1879,11 +1854,10 @@
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="19"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="19"/>
     </row>
-    <row r="14" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1900,11 +1874,10 @@
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="19"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="19"/>
     </row>
-    <row r="15" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1921,11 +1894,10 @@
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
       <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="19"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="19"/>
     </row>
-    <row r="16" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -1942,227 +1914,223 @@
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="19"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="19"/>
     </row>
-    <row r="18" spans="1:20" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="65" t="s">
+    <row r="18" spans="1:19" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="S18" s="6"/>
-    </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="67"/>
-      <c r="K19" s="68"/>
+      <c r="C19" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="68"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="L19" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O19" s="1" t="s">
+      <c r="N19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="R19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:19" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="71"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="90" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20" s="77"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="R20" s="77"/>
+      <c r="S20" s="77"/>
+    </row>
+    <row r="21" spans="1:19" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="81"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="O21" s="84"/>
+      <c r="Q21" s="85" t="s">
+        <v>64</v>
+      </c>
+      <c r="R21" s="85"/>
+      <c r="S21" s="85"/>
+    </row>
+    <row r="22" spans="1:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="81"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="88" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="88"/>
+      <c r="N22" s="14" t="s">
         <v>60</v>
       </c>
+      <c r="O22" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="R22" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="S22" s="73"/>
     </row>
-    <row r="20" spans="1:20" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="70"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="89" t="s">
-        <v>78</v>
-      </c>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
-      <c r="T20" s="76"/>
-    </row>
-    <row r="21" spans="1:20" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="79" t="s">
-        <v>47</v>
-      </c>
-      <c r="J21" s="80"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="P21" s="83"/>
-      <c r="R21" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="S21" s="84"/>
-      <c r="T21" s="84"/>
-    </row>
-    <row r="22" spans="1:20" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="8" t="s">
+    <row r="23" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="8" t="s">
+      <c r="B23" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="79" t="s">
+      <c r="H23" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="J22" s="80"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="M22" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="N22" s="87"/>
-      <c r="O22" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="P22" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="R22" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="S22" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="T22" s="72"/>
-    </row>
-    <row r="23" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="74"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="I22:K22"/>
+  <mergeCells count="41">
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:K23"/>
     <mergeCell ref="L22:L23"/>
     <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="N20:O20"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="O4:R4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2171,18 +2139,16 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="P3:R3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>